<commit_message>
[17:00 06/04/2022] ahora esta corregido ADD: por añadir display 7 de 4 seg
</commit_message>
<xml_diff>
--- a/DISPLAY_CODIFICACION.xlsx
+++ b/DISPLAY_CODIFICACION.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="26">
   <si>
     <t>Comun</t>
   </si>
@@ -132,7 +132,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -164,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -174,6 +174,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -353,6 +356,64 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>526676</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>145676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>280147</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4" descr="Display 7 Segmentos, Ánodo Común- 4 Digitos - MINI CNC ..."/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="526676" y="15576176"/>
+          <a:ext cx="2801471" cy="2801471"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100" cap="sq">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="43000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -623,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:O44"/>
+  <dimension ref="C1:O96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G80" sqref="G80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,50 +712,50 @@
       </c>
     </row>
     <row r="3" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
     </row>
     <row r="7" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
     </row>
     <row r="8" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
     </row>
     <row r="9" spans="3:15" x14ac:dyDescent="0.25">
       <c r="F9" s="1" t="s">
@@ -1049,50 +1110,50 @@
       </c>
     </row>
     <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
     </row>
     <row r="30" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
-      <c r="J30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
     </row>
     <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
     </row>
     <row r="33" spans="6:15" x14ac:dyDescent="0.25">
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
     </row>
     <row r="34" spans="6:15" x14ac:dyDescent="0.25">
       <c r="F34" s="1" t="s">
@@ -1446,12 +1507,389 @@
         <v>10</v>
       </c>
     </row>
+    <row r="84" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F84" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="6"/>
+      <c r="K84" s="6"/>
+      <c r="L84" s="6"/>
+      <c r="M84" s="6"/>
+      <c r="N84" s="6"/>
+    </row>
+    <row r="85" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
+      <c r="L85" s="6"/>
+      <c r="M85" s="6"/>
+      <c r="N85" s="6"/>
+    </row>
+    <row r="86" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F86" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J86" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K86" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="L86" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M86" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="N86" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="O86" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F87" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G87" s="3">
+        <v>0</v>
+      </c>
+      <c r="H87" s="3">
+        <v>1</v>
+      </c>
+      <c r="I87" s="3">
+        <v>0</v>
+      </c>
+      <c r="J87" s="3">
+        <v>0</v>
+      </c>
+      <c r="K87" s="3">
+        <v>0</v>
+      </c>
+      <c r="L87" s="3">
+        <v>0</v>
+      </c>
+      <c r="M87" s="3">
+        <v>0</v>
+      </c>
+      <c r="N87" s="3">
+        <v>0</v>
+      </c>
+      <c r="O87" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="88" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F88" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G88" s="3">
+        <v>1</v>
+      </c>
+      <c r="H88" s="3">
+        <v>1</v>
+      </c>
+      <c r="I88" s="3">
+        <v>1</v>
+      </c>
+      <c r="J88" s="3">
+        <v>1</v>
+      </c>
+      <c r="K88" s="3">
+        <v>1</v>
+      </c>
+      <c r="L88" s="3">
+        <v>0</v>
+      </c>
+      <c r="M88" s="3">
+        <v>0</v>
+      </c>
+      <c r="N88" s="3">
+        <v>1</v>
+      </c>
+      <c r="O88" s="3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="89" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F89" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G89" s="3">
+        <v>2</v>
+      </c>
+      <c r="H89" s="3">
+        <v>0</v>
+      </c>
+      <c r="I89" s="3">
+        <v>1</v>
+      </c>
+      <c r="J89" s="3">
+        <v>0</v>
+      </c>
+      <c r="K89" s="3">
+        <v>0</v>
+      </c>
+      <c r="L89" s="3">
+        <v>1</v>
+      </c>
+      <c r="M89" s="3">
+        <v>0</v>
+      </c>
+      <c r="N89" s="3">
+        <v>0</v>
+      </c>
+      <c r="O89" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="90" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F90" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G90" s="3">
+        <v>3</v>
+      </c>
+      <c r="H90" s="3">
+        <v>0</v>
+      </c>
+      <c r="I90" s="3">
+        <v>1</v>
+      </c>
+      <c r="J90" s="3">
+        <v>1</v>
+      </c>
+      <c r="K90" s="3">
+        <v>0</v>
+      </c>
+      <c r="L90" s="3">
+        <v>0</v>
+      </c>
+      <c r="M90" s="3">
+        <v>0</v>
+      </c>
+      <c r="N90" s="3">
+        <v>0</v>
+      </c>
+      <c r="O90" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="91" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F91" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G91" s="3">
+        <v>4</v>
+      </c>
+      <c r="H91" s="3">
+        <v>0</v>
+      </c>
+      <c r="I91" s="3">
+        <v>0</v>
+      </c>
+      <c r="J91" s="3">
+        <v>1</v>
+      </c>
+      <c r="K91" s="3">
+        <v>1</v>
+      </c>
+      <c r="L91" s="3">
+        <v>0</v>
+      </c>
+      <c r="M91" s="3">
+        <v>0</v>
+      </c>
+      <c r="N91" s="3">
+        <v>1</v>
+      </c>
+      <c r="O91" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="92" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F92" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G92" s="3">
+        <v>5</v>
+      </c>
+      <c r="H92" s="3">
+        <v>0</v>
+      </c>
+      <c r="I92" s="3">
+        <v>0</v>
+      </c>
+      <c r="J92" s="3">
+        <v>1</v>
+      </c>
+      <c r="K92" s="3">
+        <v>0</v>
+      </c>
+      <c r="L92" s="3">
+        <v>0</v>
+      </c>
+      <c r="M92" s="3">
+        <v>1</v>
+      </c>
+      <c r="N92" s="3">
+        <v>0</v>
+      </c>
+      <c r="O92" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="93" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F93" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G93" s="3">
+        <v>6</v>
+      </c>
+      <c r="H93" s="3">
+        <v>0</v>
+      </c>
+      <c r="I93" s="3">
+        <v>0</v>
+      </c>
+      <c r="J93" s="3">
+        <v>0</v>
+      </c>
+      <c r="K93" s="3">
+        <v>0</v>
+      </c>
+      <c r="L93" s="3">
+        <v>0</v>
+      </c>
+      <c r="M93" s="3">
+        <v>1</v>
+      </c>
+      <c r="N93" s="3">
+        <v>0</v>
+      </c>
+      <c r="O93" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="94" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F94" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G94" s="3">
+        <v>7</v>
+      </c>
+      <c r="H94" s="3">
+        <v>1</v>
+      </c>
+      <c r="I94" s="3">
+        <v>1</v>
+      </c>
+      <c r="J94" s="3">
+        <v>1</v>
+      </c>
+      <c r="K94" s="3">
+        <v>1</v>
+      </c>
+      <c r="L94" s="3">
+        <v>0</v>
+      </c>
+      <c r="M94" s="3">
+        <v>0</v>
+      </c>
+      <c r="N94" s="3">
+        <v>0</v>
+      </c>
+      <c r="O94" s="3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="95" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F95" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G95" s="3">
+        <v>8</v>
+      </c>
+      <c r="H95" s="3">
+        <v>0</v>
+      </c>
+      <c r="I95" s="3">
+        <v>0</v>
+      </c>
+      <c r="J95" s="3">
+        <v>0</v>
+      </c>
+      <c r="K95" s="3">
+        <v>0</v>
+      </c>
+      <c r="L95" s="3">
+        <v>0</v>
+      </c>
+      <c r="M95" s="3">
+        <v>0</v>
+      </c>
+      <c r="N95" s="3">
+        <v>0</v>
+      </c>
+      <c r="O95" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="6:15" x14ac:dyDescent="0.25">
+      <c r="F96" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G96" s="3">
+        <v>9</v>
+      </c>
+      <c r="H96" s="3">
+        <v>0</v>
+      </c>
+      <c r="I96" s="3">
+        <v>0</v>
+      </c>
+      <c r="J96" s="3">
+        <v>1</v>
+      </c>
+      <c r="K96" s="3">
+        <v>0</v>
+      </c>
+      <c r="L96" s="3">
+        <v>0</v>
+      </c>
+      <c r="M96" s="3">
+        <v>0</v>
+      </c>
+      <c r="N96" s="3">
+        <v>0</v>
+      </c>
+      <c r="O96" s="3">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C3:J4"/>
     <mergeCell ref="F7:N8"/>
     <mergeCell ref="F32:N33"/>
     <mergeCell ref="C29:J30"/>
+    <mergeCell ref="F84:N85"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>